<commit_message>
Agregar fotos en excel dignidades
</commit_message>
<xml_diff>
--- a/assets/DIGNIDADES.xlsx
+++ b/assets/DIGNIDADES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESPE\Vinculacion\Desarrollo\votaciones-backend\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESPE\SEXTO SEMESTRE\VINCULACION\github\votaciones-backend\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3367475E-E50A-4DBA-885A-D14097A6C95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB42CF-D6D5-4306-9297-43224F01A6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2760" windowWidth="29040" windowHeight="15720" xr2:uid="{6350D3E0-2AF8-4AA8-BA6F-DE5DDDF5EA10}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6350D3E0-2AF8-4AA8-BA6F-DE5DDDF5EA10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>codigoDignidad</t>
   </si>
@@ -60,13 +58,28 @@
   </si>
   <si>
     <t>Parlamento Andino</t>
+  </si>
+  <si>
+    <t>fotoDignidad</t>
+  </si>
+  <si>
+    <t>https://votoinformado.cne.gob.ec/assets/dignidades/binomio.png</t>
+  </si>
+  <si>
+    <t>https://votoinformado.cne.gob.ec/assets/dignidades/nacionales.png</t>
+  </si>
+  <si>
+    <t>https://votoinformado.cne.gob.ec/assets/dignidades/provinciales.png</t>
+  </si>
+  <si>
+    <t>https://votoinformado.cne.gob.ec/assets/dignidades/exterior.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,72 +458,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AE7625-1F61-4B89-A481-F2F47A1180E0}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.4140625" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>